<commit_message>
added facebook posts Q1
</commit_message>
<xml_diff>
--- a/Facebook Posts Q1.xlsx
+++ b/Facebook Posts Q1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tasha/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tasha/PycharmProjects/NPLF-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05FED42F-ADF7-CC42-A83A-9F12E1D0B8AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558DD4A2-F653-1E40-AE34-B9A271B9EE6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2330,7 +2330,7 @@
   <dimension ref="A1:AH57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>